<commit_message>
crawl data for season 21 22
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="52">
   <si>
     <t>Match</t>
   </si>
@@ -28,6 +28,9 @@
     <t>Home-Away</t>
   </si>
   <si>
+    <t>Competitor</t>
+  </si>
+  <si>
     <t>Manchester United v Leeds United</t>
   </si>
   <si>
@@ -125,6 +128,48 @@
   </si>
   <si>
     <t>A</t>
+  </si>
+  <si>
+    <t>Leeds United</t>
+  </si>
+  <si>
+    <t>Southampton</t>
+  </si>
+  <si>
+    <t>Wolverhampton Wanderers</t>
+  </si>
+  <si>
+    <t>Newcastle United</t>
+  </si>
+  <si>
+    <t>Young Boys Berne</t>
+  </si>
+  <si>
+    <t>West Ham United</t>
+  </si>
+  <si>
+    <t>Aston Villa</t>
+  </si>
+  <si>
+    <t>Villarreal</t>
+  </si>
+  <si>
+    <t>Everton</t>
+  </si>
+  <si>
+    <t>Leicester City</t>
+  </si>
+  <si>
+    <t>Atalanta</t>
+  </si>
+  <si>
+    <t>Liverpool</t>
+  </si>
+  <si>
+    <t>Tottenham Hotspur</t>
+  </si>
+  <si>
+    <t>Manchester City</t>
   </si>
 </sst>
 </file>
@@ -482,13 +527,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -501,277 +546,328 @@
       <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
+        <v>36</v>
+      </c>
+      <c r="F2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
+        <v>37</v>
+      </c>
+      <c r="F3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
+        <v>37</v>
+      </c>
+      <c r="F4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5" s="1">
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E5" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
+        <v>36</v>
+      </c>
+      <c r="F5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6" s="1">
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E6" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
+        <v>37</v>
+      </c>
+      <c r="F6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7" s="1">
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D7" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E7" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
+        <v>37</v>
+      </c>
+      <c r="F7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8" s="1">
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C8" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D8" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E8" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
+        <v>36</v>
+      </c>
+      <c r="F8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
       <c r="A9" s="1">
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C9" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E9" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
+        <v>36</v>
+      </c>
+      <c r="F9" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
       <c r="A10" s="1">
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C10" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D10" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E10" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
+        <v>36</v>
+      </c>
+      <c r="F10" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
       <c r="A11" s="1">
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C11" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D11" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E11" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
+        <v>36</v>
+      </c>
+      <c r="F11" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
       <c r="A12" s="1">
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C12" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D12" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E12" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
+        <v>37</v>
+      </c>
+      <c r="F12" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
       <c r="A13" s="1">
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C13" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D13" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E13" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
+        <v>36</v>
+      </c>
+      <c r="F13" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
       <c r="A14" s="1">
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D14" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E14" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5">
+        <v>36</v>
+      </c>
+      <c r="F14" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
       <c r="A15" s="1">
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C15" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D15" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E15" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5">
+        <v>37</v>
+      </c>
+      <c r="F15" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
       <c r="A16" s="1">
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C16" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D16" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E16" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5">
+        <v>37</v>
+      </c>
+      <c r="F16" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
       <c r="A17" s="1">
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C17" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D17" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E17" t="s">
-        <v>35</v>
+        <v>36</v>
+      </c>
+      <c r="F17" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>